<commit_message>
working on metabolomics example
</commit_message>
<xml_diff>
--- a/examples/metabolic_kinetics/schema.xlsx
+++ b/examples/metabolic_kinetics/schema.xlsx
@@ -4,25 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="10800"/>
+    <workbookView windowWidth="22695" windowHeight="10800"/>
   </bookViews>
   <sheets>
-    <sheet name="!!_Schema" sheetId="2" r:id="rId1"/>
+    <sheet name="!!_Schema" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Schema'!$A$2:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Schema'!$A$3:$G$57</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="107">
-  <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-05-28 23:58:52' objTablesVersion='1.0.0'</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="134">
+  <si>
+    <t>!!!ObjTables schema='schema_xbypxdpi' objTablesVersion='1.0.0' date='2020-05-28 23:58:52'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='Schema' tableFormat='row' name='schema_xbypxdpi' description='Table/model and column/attribute definitions' date='2020-05-28 23:58:52' objTablesVersion='1.0.0'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -94,6 +94,9 @@
     <t>Formula</t>
   </si>
   <si>
+    <t>A chemical formula (e.g. 'H2O', 'CO2', or 'NaCl')</t>
+  </si>
+  <si>
     <t>Reaction</t>
   </si>
   <si>
@@ -109,6 +112,9 @@
     <t>Coupled to biomass</t>
   </si>
   <si>
+    <t>Enter a Boolean value</t>
+  </si>
+  <si>
     <t>ec_number</t>
   </si>
   <si>
@@ -127,6 +133,18 @@
     <t>Equation</t>
   </si>
   <si>
+    <t>A reaction equation (e.g. 'A[c] &lt;=&gt; B[e]', '[c]: A &lt;=&gt; B')</t>
+  </si>
+  <si>
+    <t>est_range_k_ms</t>
+  </si>
+  <si>
+    <t>LongString</t>
+  </si>
+  <si>
+    <t>Estimated Km range (mM)</t>
+  </si>
+  <si>
     <t>gene_rule</t>
   </si>
   <si>
@@ -139,40 +157,97 @@
     <t>Id (iAF1260 [Ref1])</t>
   </si>
   <si>
-    <t>k_cat_k_ms</t>
+    <t>max_est_back_k_cat</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Maximum estimated backward kcat (s^-1)</t>
+  </si>
+  <si>
+    <t>max_est_for_k_cat</t>
+  </si>
+  <si>
+    <t>Maximum estimated forward kcat (s^-1)</t>
+  </si>
+  <si>
+    <t>max_obs_back_k_cat</t>
+  </si>
+  <si>
+    <t>Maximum measured backward kcat (s^-1) [Ref2, Ref3]</t>
+  </si>
+  <si>
+    <t>max_obs_for_k_cat</t>
+  </si>
+  <si>
+    <t>Maximum measured forward kcat (s^-1) [Ref2, Ref3]</t>
+  </si>
+  <si>
+    <t>min_est_back_k_cat</t>
+  </si>
+  <si>
+    <t>Minimum estimated backward kcat (s^-1)</t>
+  </si>
+  <si>
+    <t>min_est_for_k_cat</t>
+  </si>
+  <si>
+    <t>Minimum estimated forward kcat (s^-1)</t>
+  </si>
+  <si>
+    <t>min_obs_back_k_cat</t>
+  </si>
+  <si>
+    <t>Minimum measured backward kcat (s^-1) [Ref2, Ref3]</t>
+  </si>
+  <si>
+    <t>min_obs_for_k_cat</t>
+  </si>
+  <si>
+    <t>Minimum measured forward kcat (s^-1) [Ref2, Ref3]</t>
+  </si>
+  <si>
+    <t>obs_k_cat_k_ms</t>
   </si>
   <si>
     <t>ManyToMany('Kinetics', related_name='k_cat_k_m_reactions', cell_dialect='tsv')</t>
   </si>
   <si>
-    <t>kcat/Km (mM^-1 s^-1) [Ref2, Ref3]</t>
-  </si>
-  <si>
-    <t>k_cats</t>
+    <t>Measured kcat/Km (mM^-1 s^-1) [Ref2, Ref3]</t>
+  </si>
+  <si>
+    <t>obs_k_cats</t>
   </si>
   <si>
     <t>ManyToMany('Kinetics', related_name='k_cat_reactions', cell_dialect='tsv')</t>
   </si>
   <si>
-    <t>kcat (s^-1) [Ref2, Ref3]</t>
-  </si>
-  <si>
-    <t>k_is</t>
+    <t>Measured kcat (s^-1) [Ref2, Ref3]</t>
+  </si>
+  <si>
+    <t>obs_k_is</t>
   </si>
   <si>
     <t>ManyToMany('Kinetics', related_name='k_i_reactions', cell_dialect='tsv')</t>
   </si>
   <si>
-    <t>Ki (mM) [Ref2, Ref3]</t>
-  </si>
-  <si>
-    <t>k_ms</t>
+    <t>Measured Ki (mM) [Ref2, Ref3]</t>
+  </si>
+  <si>
+    <t>obs_k_ms</t>
   </si>
   <si>
     <t>ManyToMany('Kinetics', related_name='k_m_reactions', cell_dialect='tsv')</t>
   </si>
   <si>
-    <t>Km (mM) [Ref2, Ref3]</t>
+    <t>Measured Km (mM) [Ref2, Ref3]</t>
+  </si>
+  <si>
+    <t>obs_range_k_ms</t>
+  </si>
+  <si>
+    <t>Measured Km range (mM) [Ref2, Ref3]</t>
   </si>
   <si>
     <t>reversible</t>
@@ -196,9 +271,6 @@
     <t>authors</t>
   </si>
   <si>
-    <t>LongString</t>
-  </si>
-  <si>
     <t>Authors</t>
   </si>
   <si>
@@ -280,7 +352,7 @@
     <t>type</t>
   </si>
   <si>
-    <t>Enum([('activation', 1), ('competitive inhibition', 2), ('mixed inhibition', 3)])</t>
+    <t>Enum([('activation', 'activation'), ('competitive inhibition', 'competitive inhibition'), ('mixed inhibition', 'mixed inhibition')])</t>
   </si>
   <si>
     <t>Type [Ref2, Ref3]</t>
@@ -301,7 +373,7 @@
     <t>image</t>
   </si>
   <si>
-    <t>Enum([('2D-image', 1)], none=True)</t>
+    <t>Enum([('2D-image', '2D-image')], none=True)</t>
   </si>
   <si>
     <t>Image</t>
@@ -328,6 +400,9 @@
     <t>PubMed ids</t>
   </si>
   <si>
+    <t>A list of values</t>
+  </si>
+  <si>
     <t>uniprot_ids</t>
   </si>
   <si>
@@ -341,6 +416,9 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>A range of values</t>
   </si>
 </sst>
 </file>
@@ -383,9 +461,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,25 +514,56 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -428,9 +574,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -451,74 +597,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -547,37 +625,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,85 +787,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,55 +799,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -765,6 +843,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -795,26 +882,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -832,6 +899,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -841,145 +919,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1057,27 +1135,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="!!Compartments"/>
-      <sheetName val="!!Metabolites"/>
-      <sheetName val="!!Reactions"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="!!References"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1365,10 +1422,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -1391,178 +1448,172 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" customHeight="1" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" customHeight="1" spans="1:7">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:7">
-      <c r="A3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3"/>
     </row>
     <row r="4" customHeight="1" spans="1:7">
       <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" customHeight="1" spans="1:7">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" customHeight="1" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" customHeight="1" spans="1:7">
       <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" customHeight="1" spans="1:7">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" customHeight="1" spans="1:7">
       <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" customHeight="1" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" customHeight="1" spans="1:7">
@@ -1570,48 +1621,50 @@
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" customHeight="1" spans="1:7">
       <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
     </row>
     <row r="13" customHeight="1" spans="1:7">
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>33</v>
@@ -1627,127 +1680,129 @@
         <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" customHeight="1" spans="1:7">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" customHeight="1" spans="1:7">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" customHeight="1" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" customHeight="1" spans="1:7">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" customHeight="1" spans="1:7">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" customHeight="1" spans="1:7">
       <c r="A20" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>50</v>
@@ -1757,111 +1812,111 @@
     </row>
     <row r="21" customHeight="1" spans="1:7">
       <c r="A21" s="3" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" customHeight="1" spans="1:7">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" customHeight="1" spans="1:7">
       <c r="A23" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" customHeight="1" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D24" s="3" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" customHeight="1" spans="1:7">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" customHeight="1" spans="1:7">
       <c r="A26" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>62</v>
@@ -1871,19 +1926,19 @@
     </row>
     <row r="27" customHeight="1" spans="1:7">
       <c r="A27" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1893,206 +1948,208 @@
         <v>63</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" customHeight="1" spans="1:7">
       <c r="A29" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" customHeight="1" spans="1:7">
       <c r="A30" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" customHeight="1" spans="1:7">
       <c r="A31" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" customHeight="1" spans="1:7">
       <c r="A32" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" customHeight="1" spans="1:7">
       <c r="A33" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="34" customHeight="1" spans="1:7">
       <c r="A34" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D34" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" customHeight="1" spans="1:7">
       <c r="A35" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="G35" s="3"/>
     </row>
     <row r="36" customHeight="1" spans="1:7">
       <c r="A36" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" customHeight="1" spans="1:7">
       <c r="A37" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" customHeight="1" spans="1:7">
       <c r="A38" s="3" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -2102,18 +2159,18 @@
         <v>88</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="D39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" customHeight="1" spans="1:7">
@@ -2121,13 +2178,13 @@
         <v>90</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>91</v>
@@ -2140,126 +2197,341 @@
         <v>92</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
     <row r="42" customHeight="1" spans="1:7">
       <c r="A42" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" customHeight="1" spans="1:7">
       <c r="A43" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" customHeight="1" spans="1:7">
       <c r="A44" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" customHeight="1" spans="1:7">
       <c r="A45" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>88</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F45" s="3"/>
+      <c r="F45" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" customHeight="1" spans="1:7">
       <c r="A46" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
+    <row r="47" customHeight="1" spans="1:7">
+      <c r="A47" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" customHeight="1" spans="1:7">
+      <c r="A48" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" customHeight="1" spans="1:7">
+      <c r="A49" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" customHeight="1" spans="1:7">
+      <c r="A50" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" customHeight="1" spans="1:7">
+      <c r="A51" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" customHeight="1" spans="1:7">
+      <c r="A52" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" customHeight="1" spans="1:7">
+      <c r="A53" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" customHeight="1" spans="1:7">
+      <c r="A54" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" customHeight="1" spans="1:7">
+      <c r="A55" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" customHeight="1" spans="1:7">
+      <c r="A56" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" customHeight="1" spans="1:7">
+      <c r="A57" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" insertRows="0" deleteRows="0" objects="1" scenarios="1"/>
-  <autoFilter ref="A2:G46">
+  <autoFilter ref="A3:G57">
     <extLst/>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="A3" location="'!!Compartments'!A1" display="Compartment" tooltip="Click to view compartments"/>
-    <hyperlink ref="A6" location="'!!Metabolites'!A1" display="Metabolite" tooltip="Click to view metabolites"/>
-    <hyperlink ref="A10" location="'!!Reactions'!A1" display="Reaction" tooltip="Click to view reactions"/>
-    <hyperlink ref="A24" location="'!!References'!A1" display="Reference" tooltip="Click to view references"/>
-    <hyperlink ref="A34" location="'!!Regulations'!A1" display="Regulation" tooltip="Click to view regulations"/>
+    <hyperlink ref="A3" location="'!!Compartments'!A1" display="!Name" tooltip="Click to view compartments"/>
+    <hyperlink ref="A6" location="'!!Metabolites'!A1" display="name" tooltip="Click to view metabolites"/>
+    <hyperlink ref="A10" location="'!!Reactions'!A1" display="name" tooltip="Click to view reactions"/>
+    <hyperlink ref="A34" location="'!!References'!A1" display="subsystem" tooltip="Click to view references"/>
+    <hyperlink ref="A44" location="'!!Regulations'!A1" display="volume" tooltip="Click to view regulations"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>